<commit_message>
Update template download to Yesterday Stocks.xlsx
</commit_message>
<xml_diff>
--- a/Yesterday Stocks.xlsx
+++ b/Yesterday Stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Antigravity\Stock Cal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D46E449-F8A7-4466-B194-E81370334B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C166254-7979-4167-BB7B-0957FF037E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>SKU</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>RS24A17028-black-7.5</t>
+  </si>
+  <si>
+    <t>Copy your warehouse sheet data ( before updating) here. (Column C, D, E) to this sheet</t>
   </si>
 </sst>
 </file>
@@ -450,19 +453,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C610"/>
+  <dimension ref="A1:D610"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="16.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="29" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.75" customWidth="1"/>
+    <col min="4" max="4" width="86.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" customHeight="1">
+    <row r="1" spans="1:4" ht="16.5" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -471,7 +475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5" customHeight="1">
+    <row r="2" spans="1:4" ht="16.5" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -479,7 +483,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:4" ht="16.5" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -487,7 +491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" customHeight="1">
+    <row r="4" spans="1:4" ht="16.5" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -495,50 +499,53 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.5" customHeight="1">
+    <row r="5" spans="1:4" ht="16.5" customHeight="1">
       <c r="A5" s="7"/>
       <c r="B5" s="9"/>
     </row>
-    <row r="6" spans="1:3" ht="16.5" customHeight="1">
+    <row r="6" spans="1:4" ht="16.5" customHeight="1">
       <c r="A6" s="7"/>
       <c r="B6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" ht="16.5" customHeight="1">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" customHeight="1">
       <c r="A7" s="7"/>
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:3" ht="16.5" customHeight="1">
+    <row r="8" spans="1:4" ht="16.5" customHeight="1">
       <c r="A8" s="7"/>
       <c r="B8" s="9"/>
     </row>
-    <row r="9" spans="1:3" ht="16.5" customHeight="1">
+    <row r="9" spans="1:4" ht="16.5" customHeight="1">
       <c r="A9" s="7"/>
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:3" ht="16.5" customHeight="1">
+    <row r="10" spans="1:4" ht="16.5" customHeight="1">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:3" ht="16.5" customHeight="1">
+    <row r="11" spans="1:4" ht="16.5" customHeight="1">
       <c r="A11" s="7"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="16.5" customHeight="1">
+    <row r="12" spans="1:4" ht="16.5" customHeight="1">
       <c r="A12" s="7"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="16.5" customHeight="1">
+    <row r="13" spans="1:4" ht="16.5" customHeight="1">
       <c r="A13" s="7"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:3" ht="16.5" customHeight="1">
+    <row r="14" spans="1:4" ht="16.5" customHeight="1">
       <c r="A14" s="7"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:3" ht="16.5" customHeight="1">
+    <row r="15" spans="1:4" ht="16.5" customHeight="1">
       <c r="A15" s="7"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="16.5" customHeight="1">
+    <row r="16" spans="1:4" ht="16.5" customHeight="1">
       <c r="A16" s="7"/>
       <c r="B16" s="4"/>
     </row>

</xml_diff>